<commit_message>
include 稿 as anthology, fix bug for :
</commit_message>
<xml_diff>
--- a/prepare_data.xlsx
+++ b/prepare_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudos\Dropbox\create_new_books_for_cbdb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudos\Dropbox\cbdb_helpers\CBDB Programs\create-new-books-for-cbdb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5BBA46-3E31-4386-AB01-30BA10977381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DB423D-B485-440F-BA64-50BD79F32E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F58722F5-8697-4F8A-A12A-31E1AB0FB1D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F58722F5-8697-4F8A-A12A-31E1AB0FB1D1}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
   <si>
     <t>tts_sysno</t>
   </si>
@@ -113,43 +113,34 @@
     <t>c_modified_date</t>
   </si>
   <si>
-    <t>書經義要</t>
-  </si>
-  <si>
-    <t>雨餘堂集</t>
-  </si>
-  <si>
-    <t>芥溪詩集: 六卷</t>
-  </si>
-  <si>
-    <t>雜著: 四卷</t>
-  </si>
-  <si>
-    <t>周頌韻考</t>
-  </si>
-  <si>
-    <t>虛船詩文集</t>
-  </si>
-  <si>
-    <t>眉白集</t>
-  </si>
-  <si>
-    <t>周禮補選</t>
-  </si>
-  <si>
-    <t>蓉湖制藝</t>
-  </si>
-  <si>
-    <t>瑯嬛津逮</t>
-  </si>
-  <si>
-    <t>雅乘志餘</t>
-  </si>
-  <si>
-    <t>星巖集</t>
-  </si>
-  <si>
-    <t>易林補義</t>
+    <t>鄉黨圖考</t>
+  </si>
+  <si>
+    <t>詩集: 五卷</t>
+  </si>
+  <si>
+    <t>周易闡要: 三卷</t>
+  </si>
+  <si>
+    <t>蕉巖遺稿</t>
+  </si>
+  <si>
+    <t>蓮塘詩稿</t>
+  </si>
+  <si>
+    <t>元燈心法</t>
+  </si>
+  <si>
+    <t>道古堂初刻</t>
+  </si>
+  <si>
+    <t>道古齋詩稿</t>
+  </si>
+  <si>
+    <t>道古齋文稿</t>
+  </si>
+  <si>
+    <t>水經注校正</t>
   </si>
 </sst>
 </file>
@@ -502,21 +493,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA7C8E7-4B12-4E2E-BAAA-516EAC8A16B7}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="A1:C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>558382</v>
+        <v>562361</v>
       </c>
       <c r="B1" t="s">
         <v>25</v>
@@ -527,7 +517,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>558382</v>
+        <v>562361</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
@@ -538,7 +528,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>559958</v>
+        <v>562365</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
@@ -549,7 +539,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>559958</v>
+        <v>562375</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
@@ -560,7 +550,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>559959</v>
+        <v>562375</v>
       </c>
       <c r="B5" t="s">
         <v>29</v>
@@ -571,7 +561,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>559960</v>
+        <v>562375</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
@@ -582,7 +572,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>559969</v>
+        <v>72460</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
@@ -593,7 +583,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>559971</v>
+        <v>72460</v>
       </c>
       <c r="B8" t="s">
         <v>32</v>
@@ -604,7 +594,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>562356</v>
+        <v>72460</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
@@ -615,7 +605,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>562357</v>
+        <v>72460</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
@@ -624,41 +614,9 @@
         <v>57941</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>562357</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11">
-        <v>57941</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>562358</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12">
-        <v>57941</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>562359</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13">
-        <v>57941</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -666,7 +624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C53A501-6408-4EFF-A818-284A3C9C584F}">
   <dimension ref="A1:Y30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>